<commit_message>
Mejorado proveedor 70018938, formateo codigo
</commit_message>
<xml_diff>
--- a/AI_Engine/Info/Results_notes.xlsx
+++ b/AI_Engine/Info/Results_notes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proyectos\Nueva carpeta\Bot-Creacion-de-Pedidos\AI_Engine\Info\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deere-my.sharepoint.com/personal/gonzalezdiazsergio_johndeere_com/Documents/Desktop/Proyectos/Bot-Creacion-de-Pedidos/AI_Engine/Info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D98053C-0B63-4673-A049-1B2D122FE4D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{7D98053C-0B63-4673-A049-1B2D122FE4D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F05BF609-10BB-4FDD-8070-C18AD6EEE7C4}"/>
   <bookViews>
-    <workbookView xWindow="-8205" yWindow="4020" windowWidth="16995" windowHeight="10230" xr2:uid="{DD84187C-4454-4454-99E3-348581278C74}"/>
+    <workbookView xWindow="-130" yWindow="10690" windowWidth="19420" windowHeight="10420" xr2:uid="{DD84187C-4454-4454-99E3-348581278C74}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="81">
   <si>
     <t>Thyssenkrupp Crankshaft</t>
   </si>
@@ -202,9 +202,6 @@
     <t>Todo igual. Probar a usar multiple ocr en Order number</t>
   </si>
   <si>
-    <t>4445 mejora regex</t>
-  </si>
-  <si>
     <t>Checkear valores otra vez. Mejora notable respecto a fechas, pero siguen quedando algunas</t>
   </si>
   <si>
@@ -248,6 +245,39 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>5554 mejora regex</t>
+  </si>
+  <si>
+    <t>5555</t>
+  </si>
+  <si>
+    <t>555[4,5] agrandamiento roi</t>
+  </si>
+  <si>
+    <t>65/65</t>
+  </si>
+  <si>
+    <t>Deteccion mejora. Arreglo de qty que no habia visto. Como inconveniente tarda algo más</t>
+  </si>
+  <si>
+    <t>80,29</t>
+  </si>
+  <si>
+    <t>[4,7]747</t>
+  </si>
+  <si>
+    <t>85,18</t>
+  </si>
+  <si>
+    <t>667/667</t>
+  </si>
+  <si>
+    <t>Valores al revés, revisar</t>
+  </si>
+  <si>
+    <t>[4,7]477</t>
   </si>
 </sst>
 </file>
@@ -271,7 +301,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -290,6 +320,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -428,7 +464,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -467,21 +503,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -493,12 +514,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -506,9 +521,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -523,6 +535,27 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -532,9 +565,26 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -851,8 +901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F69B5C2-6A59-4267-B787-FDE4B635DD6F}">
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" topLeftCell="B34" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,15 +920,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="26" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="27"/>
+      <c r="E1" s="43"/>
       <c r="F1" s="17"/>
       <c r="G1" s="18"/>
       <c r="H1" s="17"/>
@@ -890,10 +940,10 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="19"/>
-      <c r="B2" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="35" t="s">
+      <c r="B2" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="30" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="8" t="s">
@@ -913,10 +963,10 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
-      <c r="B3" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="35" t="s">
+      <c r="B3" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="30" t="s">
         <v>31</v>
       </c>
       <c r="D3" s="8" t="s">
@@ -936,10 +986,10 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
-      <c r="B4" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="35" t="s">
+      <c r="B4" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="30" t="s">
         <v>32</v>
       </c>
       <c r="D4" s="8" t="s">
@@ -959,10 +1009,10 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="20"/>
-      <c r="B5" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="37" t="s">
+      <c r="B5" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="32" t="s">
         <v>33</v>
       </c>
       <c r="D5" s="9" t="s">
@@ -981,15 +1031,15 @@
       <c r="M5" s="16"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="26" t="s">
+      <c r="B6" s="27"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="27"/>
+      <c r="E6" s="43"/>
       <c r="F6" s="17"/>
       <c r="G6" s="18"/>
       <c r="H6" s="17"/>
@@ -1001,10 +1051,10 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
-      <c r="B7" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="35" t="s">
+      <c r="B7" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="30" t="s">
         <v>37</v>
       </c>
       <c r="D7" s="8" t="s">
@@ -1024,10 +1074,10 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="19"/>
-      <c r="B8" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="35" t="s">
+      <c r="B8" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="30" t="s">
         <v>38</v>
       </c>
       <c r="D8" s="8" t="s">
@@ -1047,10 +1097,10 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="19"/>
-      <c r="B9" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="35" t="s">
+      <c r="B9" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="30" t="s">
         <v>39</v>
       </c>
       <c r="D9" s="8" t="s">
@@ -1070,10 +1120,10 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="19"/>
-      <c r="B10" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="35"/>
+      <c r="B10" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="30"/>
       <c r="D10" s="8" t="s">
         <v>8</v>
       </c>
@@ -1088,15 +1138,15 @@
       <c r="M10" s="15"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="32"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="39" t="s">
+      <c r="B11" s="27"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="43"/>
+      <c r="E11" s="45"/>
       <c r="F11" s="17"/>
       <c r="G11" s="18"/>
       <c r="H11" s="17"/>
@@ -1108,16 +1158,16 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="19"/>
-      <c r="B12" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="35" t="s">
+      <c r="B12" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="44" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="45" t="s">
+      <c r="D12" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="37" t="s">
         <v>41</v>
       </c>
       <c r="F12" s="2"/>
@@ -1131,16 +1181,16 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="19"/>
-      <c r="B13" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="35" t="s">
+      <c r="B13" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="45" t="s">
+      <c r="D13" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="37" t="s">
         <v>44</v>
       </c>
       <c r="F13" s="2"/>
@@ -1154,16 +1204,16 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="19"/>
-      <c r="B14" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="35" t="s">
+      <c r="B14" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="45" t="s">
+      <c r="D14" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="37" t="s">
         <v>52</v>
       </c>
       <c r="F14" s="2" t="s">
@@ -1179,14 +1229,14 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="20"/>
-      <c r="B15" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="47" t="s">
+      <c r="B15" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="32"/>
+      <c r="D15" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="39" t="s">
         <v>43</v>
       </c>
       <c r="F15" s="5"/>
@@ -1199,15 +1249,15 @@
       <c r="M15" s="16"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="26" t="s">
+      <c r="B16" s="27"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="27"/>
+      <c r="E16" s="43"/>
       <c r="F16" s="17"/>
       <c r="G16" s="18"/>
       <c r="H16" s="17"/>
@@ -1219,10 +1269,10 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
-      <c r="B17" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="35" t="s">
+      <c r="B17" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="30" t="s">
         <v>46</v>
       </c>
       <c r="D17" s="8" t="s">
@@ -1242,10 +1292,10 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="19"/>
-      <c r="B18" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="35" t="s">
+      <c r="B18" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="30" t="s">
         <v>47</v>
       </c>
       <c r="D18" s="8" t="s">
@@ -1265,10 +1315,10 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="19"/>
-      <c r="B19" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="35" t="s">
+      <c r="B19" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="30" t="s">
         <v>48</v>
       </c>
       <c r="D19" s="8" t="s">
@@ -1288,15 +1338,15 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="19"/>
-      <c r="B20" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="35"/>
+      <c r="B20" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="30"/>
       <c r="D20" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="15"/>
@@ -1308,25 +1358,25 @@
       <c r="M20" s="15"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="38">
+      <c r="B21" s="47">
         <v>4444</v>
       </c>
-      <c r="C21" s="39"/>
-      <c r="D21" s="38">
+      <c r="C21" s="44"/>
+      <c r="D21" s="47">
         <v>5444</v>
       </c>
-      <c r="E21" s="38"/>
-      <c r="F21" s="28" t="s">
+      <c r="E21" s="47"/>
+      <c r="F21" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="G21" s="28"/>
-      <c r="H21" s="26" t="s">
+      <c r="G21" s="48"/>
+      <c r="H21" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="I21" s="27"/>
+      <c r="I21" s="43"/>
       <c r="J21" s="17"/>
       <c r="K21" s="18"/>
       <c r="L21" s="17"/>
@@ -1334,16 +1384,16 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="19"/>
-      <c r="B22" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="40">
+      <c r="B22" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="33">
         <v>12</v>
       </c>
-      <c r="D22" s="44" t="s">
-        <v>5</v>
-      </c>
-      <c r="E22" s="48">
+      <c r="D22" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="40">
         <v>12</v>
       </c>
       <c r="F22" s="8" t="s">
@@ -1365,16 +1415,16 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="19"/>
-      <c r="B23" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="40">
+      <c r="B23" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="33">
         <v>90.02</v>
       </c>
-      <c r="D23" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="E23" s="48">
+      <c r="D23" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="40">
         <v>90.29</v>
       </c>
       <c r="F23" s="8" t="s">
@@ -1396,16 +1446,16 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
-      <c r="B24" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="40" t="s">
+      <c r="B24" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="D24" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="48" t="s">
+      <c r="D24" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="40" t="s">
         <v>3</v>
       </c>
       <c r="F24" s="8" t="s">
@@ -1427,16 +1477,16 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="20"/>
-      <c r="B25" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="41" t="s">
+      <c r="B25" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="D25" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="49" t="s">
+      <c r="D25" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="41" t="s">
         <v>4</v>
       </c>
       <c r="F25" s="9" t="s">
@@ -1457,17 +1507,21 @@
       <c r="M25" s="16"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="31" t="s">
+      <c r="A26" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="32"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="39" t="s">
-        <v>55</v>
-      </c>
-      <c r="E26" s="43"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="18"/>
+      <c r="B26" s="44" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" s="45"/>
+      <c r="D26" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="E26" s="45"/>
+      <c r="F26" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="G26" s="43"/>
       <c r="H26" s="17"/>
       <c r="I26" s="18"/>
       <c r="J26" s="17"/>
@@ -1477,20 +1531,24 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
-      <c r="B27" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="42" t="s">
+      <c r="B27" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="44" t="s">
-        <v>5</v>
-      </c>
-      <c r="E27" s="45" t="s">
+      <c r="D27" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="F27" s="2"/>
-      <c r="G27" s="15"/>
+      <c r="F27" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>26</v>
+      </c>
       <c r="H27" s="2"/>
       <c r="I27" s="15"/>
       <c r="J27" s="2"/>
@@ -1500,20 +1558,24 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="19"/>
-      <c r="B28" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" s="42" t="s">
+      <c r="B28" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28" s="45" t="s">
+      <c r="D28" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="F28" s="2"/>
-      <c r="G28" s="15"/>
+      <c r="F28" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>75</v>
+      </c>
       <c r="H28" s="2"/>
       <c r="I28" s="15"/>
       <c r="J28" s="2"/>
@@ -1523,20 +1585,24 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="19"/>
-      <c r="B29" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="42" t="s">
+      <c r="B29" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="D29" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" s="45" t="s">
+      <c r="D29" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="F29" s="2"/>
-      <c r="G29" s="15"/>
+      <c r="F29" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>73</v>
+      </c>
       <c r="H29" s="2"/>
       <c r="I29" s="15"/>
       <c r="J29" s="2"/>
@@ -1546,20 +1612,24 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="19"/>
-      <c r="B30" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="42" t="s">
+      <c r="B30" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" s="45" t="s">
-        <v>56</v>
-      </c>
-      <c r="F30" s="2"/>
-      <c r="G30" s="15"/>
+      <c r="D30" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>74</v>
+      </c>
       <c r="H30" s="2"/>
       <c r="I30" s="15"/>
       <c r="J30" s="2"/>
@@ -1568,15 +1638,15 @@
       <c r="M30" s="15"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="31" t="s">
-        <v>57</v>
+      <c r="A31" s="26" t="s">
+        <v>56</v>
       </c>
       <c r="B31" s="24"/>
       <c r="C31" s="25"/>
-      <c r="D31" s="39" t="s">
+      <c r="D31" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="E31" s="43"/>
+      <c r="E31" s="55"/>
       <c r="F31" s="17"/>
       <c r="G31" s="18"/>
       <c r="H31" s="17"/>
@@ -1592,13 +1662,13 @@
         <v>5</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="D32" s="44" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32" s="45" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="D32" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="57" t="s">
+        <v>58</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="15"/>
@@ -1615,13 +1685,13 @@
         <v>6</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D33" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="E33" s="45" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+      <c r="D33" s="56" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="57" t="s">
+        <v>59</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="15"/>
@@ -1638,13 +1708,13 @@
         <v>7</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="D34" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="E34" s="45" t="s">
-        <v>61</v>
+        <v>60</v>
+      </c>
+      <c r="D34" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="57" t="s">
+        <v>60</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="15"/>
@@ -1661,11 +1731,11 @@
         <v>8</v>
       </c>
       <c r="C35" s="22"/>
-      <c r="D35" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="E35" s="47" t="s">
-        <v>58</v>
+      <c r="D35" s="58" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="59" t="s">
+        <v>57</v>
       </c>
       <c r="F35" s="5"/>
       <c r="G35" s="16"/>
@@ -1677,19 +1747,19 @@
       <c r="M35" s="16"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="31" t="s">
+      <c r="A36" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="50"/>
-      <c r="C36" s="50"/>
-      <c r="D36" s="51" t="s">
+      <c r="B36" s="49"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="E36" s="52"/>
-      <c r="F36" s="29" t="s">
+      <c r="E36" s="51"/>
+      <c r="F36" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="G36" s="30"/>
+      <c r="G36" s="53"/>
       <c r="H36" s="2"/>
       <c r="I36" s="15"/>
       <c r="J36" s="2"/>
@@ -1699,16 +1769,16 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="19"/>
-      <c r="B37" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" s="35">
-        <v>8</v>
-      </c>
-      <c r="D37" s="44" t="s">
-        <v>5</v>
-      </c>
-      <c r="E37" s="45" t="s">
+      <c r="B37" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="30">
+        <v>8</v>
+      </c>
+      <c r="D37" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="37" t="s">
         <v>17</v>
       </c>
       <c r="F37" s="8" t="s">
@@ -1726,16 +1796,16 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="19"/>
-      <c r="B38" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="C38" s="35" t="s">
+      <c r="B38" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="D38" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="E38" s="45" t="s">
+      <c r="D38" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" s="37" t="s">
         <v>18</v>
       </c>
       <c r="F38" s="8" t="s">
@@ -1753,16 +1823,16 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="19"/>
-      <c r="B39" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" s="35" t="s">
+      <c r="B39" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="D39" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="E39" s="45" t="s">
+      <c r="D39" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="37" t="s">
         <v>14</v>
       </c>
       <c r="F39" s="8" t="s">
@@ -1780,16 +1850,16 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="19"/>
-      <c r="B40" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="C40" s="35" t="s">
+      <c r="B40" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="D40" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="E40" s="45" t="s">
+      <c r="D40" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="37" t="s">
         <v>22</v>
       </c>
       <c r="F40" s="8" t="s">
@@ -1806,19 +1876,23 @@
       <c r="M40" s="15"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="B41" s="39"/>
-      <c r="C41" s="53"/>
-      <c r="D41" s="39" t="s">
+      <c r="A41" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="B41" s="44"/>
+      <c r="C41" s="46"/>
+      <c r="D41" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="E41" s="43"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="18"/>
-      <c r="H41" s="17"/>
-      <c r="I41" s="18"/>
+      <c r="E41" s="45"/>
+      <c r="F41" s="54" t="s">
+        <v>76</v>
+      </c>
+      <c r="G41" s="55"/>
+      <c r="H41" s="54" t="s">
+        <v>80</v>
+      </c>
+      <c r="I41" s="55"/>
       <c r="J41" s="17"/>
       <c r="K41" s="18"/>
       <c r="L41" s="17"/>
@@ -1826,22 +1900,30 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="19"/>
-      <c r="B42" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C42" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="D42" s="44" t="s">
-        <v>5</v>
-      </c>
-      <c r="E42" s="45" t="s">
-        <v>63</v>
-      </c>
-      <c r="F42" s="2"/>
-      <c r="G42" s="15"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="15"/>
+      <c r="B42" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="D42" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="E42" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="F42" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="G42" s="57" t="s">
+        <v>62</v>
+      </c>
+      <c r="H42" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="I42" s="57" t="s">
+        <v>62</v>
+      </c>
       <c r="J42" s="2"/>
       <c r="K42" s="15"/>
       <c r="L42" s="2"/>
@@ -1849,22 +1931,30 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="19"/>
-      <c r="B43" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="C43" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="D43" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="E43" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="F43" s="2"/>
-      <c r="G43" s="15"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="15"/>
+      <c r="B43" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="D43" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="F43" s="56" t="s">
+        <v>6</v>
+      </c>
+      <c r="G43" s="57" t="s">
+        <v>77</v>
+      </c>
+      <c r="H43" s="56" t="s">
+        <v>6</v>
+      </c>
+      <c r="I43" s="57" t="s">
+        <v>77</v>
+      </c>
       <c r="J43" s="2"/>
       <c r="K43" s="15"/>
       <c r="L43" s="2"/>
@@ -1872,22 +1962,30 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="19"/>
-      <c r="B44" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="C44" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="D44" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="E44" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="F44" s="2"/>
-      <c r="G44" s="15"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="15"/>
+      <c r="B44" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D44" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="F44" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="G44" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="H44" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="I44" s="57" t="s">
+        <v>78</v>
+      </c>
       <c r="J44" s="2"/>
       <c r="K44" s="15"/>
       <c r="L44" s="2"/>
@@ -1895,35 +1993,43 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="20"/>
-      <c r="B45" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="C45" s="37"/>
-      <c r="D45" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="E45" s="47" t="s">
-        <v>58</v>
-      </c>
-      <c r="F45" s="5"/>
-      <c r="G45" s="16"/>
-      <c r="H45" s="5"/>
-      <c r="I45" s="16"/>
+      <c r="B45" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" s="32"/>
+      <c r="D45" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="F45" s="58" t="s">
+        <v>8</v>
+      </c>
+      <c r="G45" s="59" t="s">
+        <v>79</v>
+      </c>
+      <c r="H45" s="58" t="s">
+        <v>8</v>
+      </c>
+      <c r="I45" s="59" t="s">
+        <v>79</v>
+      </c>
       <c r="J45" s="5"/>
       <c r="K45" s="16"/>
       <c r="L45" s="5"/>
       <c r="M45" s="16"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" s="31" t="s">
-        <v>67</v>
+      <c r="A46" s="26" t="s">
+        <v>66</v>
       </c>
       <c r="B46" s="25"/>
       <c r="C46" s="25"/>
-      <c r="D46" s="26" t="s">
+      <c r="D46" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="E46" s="27"/>
+      <c r="E46" s="43"/>
       <c r="F46" s="17"/>
       <c r="G46" s="18"/>
       <c r="H46" s="23"/>
@@ -1939,13 +2045,13 @@
         <v>5</v>
       </c>
       <c r="C47" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D47" s="8" t="s">
         <v>5</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F47" s="2"/>
       <c r="G47" s="15"/>
@@ -1962,13 +2068,13 @@
         <v>6</v>
       </c>
       <c r="C48" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F48" s="2"/>
       <c r="G48" s="15"/>
@@ -1985,13 +2091,13 @@
         <v>7</v>
       </c>
       <c r="C49" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D49" s="8" t="s">
         <v>7</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F49" s="2"/>
       <c r="G49" s="15"/>
@@ -2026,23 +2132,27 @@
       <c r="M50" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="20">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D21:E21"/>
     <mergeCell ref="D46:E46"/>
     <mergeCell ref="H21:I21"/>
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D26:E26"/>
     <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
     <mergeCell ref="F21:G21"/>
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="D36:E36"/>
     <mergeCell ref="F36:G36"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="H41:I41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>

</xml_diff>

<commit_message>
Cambiado configuracion para mayor conf
</commit_message>
<xml_diff>
--- a/AI_Engine/Info/Results_notes.xlsx
+++ b/AI_Engine/Info/Results_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deere-my.sharepoint.com/personal/gonzalezdiazsergio_johndeere_com/Documents/Desktop/Proyectos/Bot-Creacion-de-Pedidos/AI_Engine/Info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{7D98053C-0B63-4673-A049-1B2D122FE4D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F05BF609-10BB-4FDD-8070-C18AD6EEE7C4}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:1_{7D98053C-0B63-4673-A049-1B2D122FE4D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2116BAC9-9402-47F1-85A4-F2E16E50A489}"/>
   <bookViews>
     <workbookView xWindow="-130" yWindow="10690" windowWidth="19420" windowHeight="10420" xr2:uid="{DD84187C-4454-4454-99E3-348581278C74}"/>
   </bookViews>
@@ -35,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="81">
-  <si>
-    <t>Thyssenkrupp Crankshaft</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="100">
   <si>
     <t>62/148</t>
   </si>
@@ -73,9 +70,6 @@
     <t>Probar a usar multiple ocr en Order number</t>
   </si>
   <si>
-    <t>TIG</t>
-  </si>
-  <si>
     <t>66,9</t>
   </si>
   <si>
@@ -109,9 +103,6 @@
     <t>Preguntar por coordenadas referencia. Mejorar detección en qty</t>
   </si>
   <si>
-    <t>Thyssenkrupp Campo Limpo</t>
-  </si>
-  <si>
     <t>70,19</t>
   </si>
   <si>
@@ -124,9 +115,6 @@
     <t>Error en la validacion de fecha, coge W como WW</t>
   </si>
   <si>
-    <t>JD SARAN</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
@@ -142,9 +130,6 @@
     <t>89,50</t>
   </si>
   <si>
-    <t>JD REMAN</t>
-  </si>
-  <si>
     <t>91,69</t>
   </si>
   <si>
@@ -157,9 +142,6 @@
     <t>24/24</t>
   </si>
   <si>
-    <t>ESP</t>
-  </si>
-  <si>
     <t>33</t>
   </si>
   <si>
@@ -172,9 +154,6 @@
     <t>86,62</t>
   </si>
   <si>
-    <t>EMP</t>
-  </si>
-  <si>
     <t>41</t>
   </si>
   <si>
@@ -205,9 +184,6 @@
     <t>Checkear valores otra vez. Mejora notable respecto a fechas, pero siguen quedando algunas</t>
   </si>
   <si>
-    <t>Engine Power Components</t>
-  </si>
-  <si>
     <t>Se me ha dado la vuelta a los valores, revisar</t>
   </si>
   <si>
@@ -220,9 +196,6 @@
     <t>38/38</t>
   </si>
   <si>
-    <t>WorldClass Industries</t>
-  </si>
-  <si>
     <t>52</t>
   </si>
   <si>
@@ -235,9 +208,6 @@
     <t>se ha corregido el orden de los datos, Revisar</t>
   </si>
   <si>
-    <t>Skyway</t>
-  </si>
-  <si>
     <t>21/21</t>
   </si>
   <si>
@@ -278,6 +248,93 @@
   </si>
   <si>
     <t>[4,7]477</t>
+  </si>
+  <si>
+    <t>JD SARAN 99999TCD00</t>
+  </si>
+  <si>
+    <t>JD REMAN 99999TSE01</t>
+  </si>
+  <si>
+    <t>ESP 70001256</t>
+  </si>
+  <si>
+    <t>EMP 70012672</t>
+  </si>
+  <si>
+    <t>Thyssenkrupp Crankshaft 70017048</t>
+  </si>
+  <si>
+    <t>Thyssenkrupp Campo Limpo 70017078</t>
+  </si>
+  <si>
+    <t>Engine Power Components 70017703</t>
+  </si>
+  <si>
+    <t>TIG 70017869</t>
+  </si>
+  <si>
+    <t>WorldClass Industries 70018938</t>
+  </si>
+  <si>
+    <t>Skyway 70001353</t>
+  </si>
+  <si>
+    <t>agrandamiento</t>
+  </si>
+  <si>
+    <t>91,273</t>
+  </si>
+  <si>
+    <t>44/77 (25 fechas mal porque el proveedor no lo ha puesto)</t>
+  </si>
+  <si>
+    <t>mirar</t>
+  </si>
+  <si>
+    <t>80,55</t>
+  </si>
+  <si>
+    <t>83,3</t>
+  </si>
+  <si>
+    <t>89,13</t>
+  </si>
+  <si>
+    <t>86,94</t>
+  </si>
+  <si>
+    <t>Aconsejo juntar ocrs, ver en qué campos es mejor</t>
+  </si>
+  <si>
+    <t>90,59</t>
+  </si>
+  <si>
+    <t>Preguntar por coordenadas referencia</t>
+  </si>
+  <si>
+    <t>87,94</t>
+  </si>
+  <si>
+    <t>Mejora conf, pero no se aplica porque agrada el 7</t>
+  </si>
+  <si>
+    <t>89,25</t>
+  </si>
+  <si>
+    <t>En el registro de menor conf (69), ha bajado a 68, mientras ha subido en los demás. Necesitamos más proveedores</t>
+  </si>
+  <si>
+    <t>777[7,8] agrandamiento</t>
+  </si>
+  <si>
+    <t>Algo raro, probar 888[7,8]</t>
+  </si>
+  <si>
+    <t>0000 agrandamiento</t>
+  </si>
+  <si>
+    <t>91,41</t>
   </si>
 </sst>
 </file>
@@ -301,7 +358,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -323,6 +380,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -464,7 +527,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -535,48 +598,6 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -585,6 +606,62 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -901,13 +978,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F69B5C2-6A59-4267-B787-FDE4B635DD6F}">
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B34" workbookViewId="0">
-      <selection activeCell="H48" sqref="H48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5703125" style="10" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -916,21 +993,24 @@
     <col min="7" max="7" width="19.7109375" style="1" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.42578125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="1"/>
+    <col min="10" max="10" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
-        <v>29</v>
+        <v>71</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="28"/>
-      <c r="D1" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="43"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="18"/>
+      <c r="D1" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="47"/>
+      <c r="F1" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="47"/>
       <c r="H1" s="17"/>
       <c r="I1" s="18"/>
       <c r="J1" s="17"/>
@@ -941,19 +1021,23 @@
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="19"/>
       <c r="B2" s="29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="15"/>
+        <v>26</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>26</v>
+      </c>
       <c r="H2" s="2"/>
       <c r="I2" s="15"/>
       <c r="J2" s="2"/>
@@ -964,19 +1048,23 @@
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
       <c r="B3" s="29" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="15"/>
+        <v>30</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>82</v>
+      </c>
       <c r="H3" s="2"/>
       <c r="I3" s="15"/>
       <c r="J3" s="2"/>
@@ -987,19 +1075,23 @@
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
       <c r="B4" s="29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="15"/>
+        <v>28</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>28</v>
+      </c>
       <c r="H4" s="2"/>
       <c r="I4" s="15"/>
       <c r="J4" s="2"/>
@@ -1010,19 +1102,23 @@
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="20"/>
       <c r="B5" s="31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="16"/>
+        <v>29</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>29</v>
+      </c>
       <c r="H5" s="5"/>
       <c r="I5" s="16"/>
       <c r="J5" s="5"/>
@@ -1032,16 +1128,18 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
-        <v>35</v>
+        <v>72</v>
       </c>
       <c r="B6" s="27"/>
       <c r="C6" s="28"/>
-      <c r="D6" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="43"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="18"/>
+      <c r="D6" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="47"/>
+      <c r="F6" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="G6" s="52"/>
       <c r="H6" s="17"/>
       <c r="I6" s="18"/>
       <c r="J6" s="17"/>
@@ -1052,19 +1150,23 @@
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
       <c r="B7" s="29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="15"/>
+        <v>32</v>
+      </c>
+      <c r="F7" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="43" t="s">
+        <v>32</v>
+      </c>
       <c r="H7" s="2"/>
       <c r="I7" s="15"/>
       <c r="J7" s="2"/>
@@ -1075,19 +1177,23 @@
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="19"/>
       <c r="B8" s="29" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="15"/>
+        <v>31</v>
+      </c>
+      <c r="F8" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="43" t="s">
+        <v>99</v>
+      </c>
       <c r="H8" s="2"/>
       <c r="I8" s="15"/>
       <c r="J8" s="2"/>
@@ -1098,19 +1204,23 @@
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="19"/>
       <c r="B9" s="29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="15"/>
+        <v>34</v>
+      </c>
+      <c r="F9" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="43" t="s">
+        <v>34</v>
+      </c>
       <c r="H9" s="2"/>
       <c r="I9" s="15"/>
       <c r="J9" s="2"/>
@@ -1121,15 +1231,17 @@
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="19"/>
       <c r="B10" s="29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="30"/>
       <c r="D10" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E10" s="12"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="15"/>
+      <c r="F10" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="43"/>
       <c r="H10" s="2"/>
       <c r="I10" s="15"/>
       <c r="J10" s="2"/>
@@ -1139,15 +1251,17 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="B11" s="27"/>
       <c r="C11" s="28"/>
-      <c r="D11" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="45"/>
-      <c r="F11" s="17"/>
+      <c r="D11" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="49"/>
+      <c r="F11" s="17" t="s">
+        <v>84</v>
+      </c>
       <c r="G11" s="18"/>
       <c r="H11" s="17"/>
       <c r="I11" s="18"/>
@@ -1159,16 +1273,16 @@
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="19"/>
       <c r="B12" s="29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D12" s="36" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="15"/>
@@ -1182,16 +1296,16 @@
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="19"/>
       <c r="B13" s="29" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D13" s="36" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E13" s="37" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="15"/>
@@ -1205,19 +1319,19 @@
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="19"/>
       <c r="B14" s="29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D14" s="36" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E14" s="37" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="G14" s="15"/>
       <c r="H14" s="2"/>
@@ -1230,14 +1344,14 @@
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="20"/>
       <c r="B15" s="31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C15" s="32"/>
       <c r="D15" s="38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E15" s="39" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="16"/>
@@ -1250,16 +1364,18 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="B16" s="27"/>
       <c r="C16" s="28"/>
-      <c r="D16" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="43"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="18"/>
+      <c r="D16" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="47"/>
+      <c r="F16" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="G16" s="52"/>
       <c r="H16" s="17"/>
       <c r="I16" s="18"/>
       <c r="J16" s="17"/>
@@ -1270,19 +1386,23 @@
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
       <c r="B17" s="29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="15"/>
+        <v>39</v>
+      </c>
+      <c r="F17" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="43" t="s">
+        <v>39</v>
+      </c>
       <c r="H17" s="2"/>
       <c r="I17" s="15"/>
       <c r="J17" s="2"/>
@@ -1293,19 +1413,23 @@
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="19"/>
       <c r="B18" s="29" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="15"/>
+        <v>40</v>
+      </c>
+      <c r="F18" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" s="43" t="s">
+        <v>85</v>
+      </c>
       <c r="H18" s="2"/>
       <c r="I18" s="15"/>
       <c r="J18" s="2"/>
@@ -1316,19 +1440,23 @@
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="19"/>
       <c r="B19" s="29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19" s="30" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="15"/>
+        <v>41</v>
+      </c>
+      <c r="F19" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="43" t="s">
+        <v>41</v>
+      </c>
       <c r="H19" s="2"/>
       <c r="I19" s="15"/>
       <c r="J19" s="2"/>
@@ -1339,17 +1467,19 @@
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="19"/>
       <c r="B20" s="29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C20" s="30"/>
       <c r="D20" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="F20" s="2"/>
-      <c r="G20" s="15"/>
+        <v>56</v>
+      </c>
+      <c r="F20" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="43"/>
       <c r="H20" s="2"/>
       <c r="I20" s="15"/>
       <c r="J20" s="2"/>
@@ -1359,171 +1489,191 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="47">
+        <v>75</v>
+      </c>
+      <c r="B21" s="50">
         <v>4444</v>
       </c>
-      <c r="C21" s="44"/>
-      <c r="D21" s="47">
+      <c r="C21" s="48"/>
+      <c r="D21" s="50">
         <v>5444</v>
       </c>
-      <c r="E21" s="47"/>
-      <c r="F21" s="48" t="s">
-        <v>9</v>
-      </c>
-      <c r="G21" s="48"/>
-      <c r="H21" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="I21" s="43"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="18"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="54" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" s="54"/>
+      <c r="H21" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="47"/>
+      <c r="J21" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="K21" s="52"/>
       <c r="L21" s="17"/>
       <c r="M21" s="18"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="19"/>
       <c r="B22" s="29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C22" s="33">
         <v>12</v>
       </c>
       <c r="D22" s="36" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E22" s="40">
         <v>12</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G22" s="4">
         <v>12</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="J22" s="2"/>
-      <c r="K22" s="15"/>
+        <v>23</v>
+      </c>
+      <c r="J22" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="K22" s="43" t="s">
+        <v>23</v>
+      </c>
       <c r="L22" s="2"/>
       <c r="M22" s="15"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="19"/>
       <c r="B23" s="29" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C23" s="33">
         <v>90.02</v>
       </c>
       <c r="D23" s="36" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E23" s="40">
         <v>90.29</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I23" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="J23" s="2"/>
-      <c r="K23" s="15"/>
+        <v>42</v>
+      </c>
+      <c r="J23" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="K23" s="43" t="s">
+        <v>86</v>
+      </c>
       <c r="L23" s="2"/>
       <c r="M23" s="15"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
       <c r="B24" s="29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C24" s="33" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24" s="36" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E24" s="40" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="J24" s="2"/>
-      <c r="K24" s="15"/>
+        <v>9</v>
+      </c>
+      <c r="J24" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="K24" s="43" t="s">
+        <v>9</v>
+      </c>
       <c r="L24" s="2"/>
       <c r="M24" s="15"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="20"/>
       <c r="B25" s="31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C25" s="34" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D25" s="38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E25" s="41" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="J25" s="5"/>
-      <c r="K25" s="16"/>
+        <v>47</v>
+      </c>
+      <c r="J25" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="K25" s="45" t="s">
+        <v>47</v>
+      </c>
       <c r="L25" s="5"/>
       <c r="M25" s="16"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="44" t="s">
-        <v>71</v>
-      </c>
-      <c r="C26" s="45"/>
-      <c r="D26" s="44" t="s">
-        <v>70</v>
-      </c>
-      <c r="E26" s="45"/>
-      <c r="F26" s="42" t="s">
-        <v>72</v>
-      </c>
-      <c r="G26" s="43"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="18"/>
+        <v>76</v>
+      </c>
+      <c r="B26" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="49"/>
+      <c r="D26" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="E26" s="49"/>
+      <c r="F26" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="G26" s="47"/>
+      <c r="H26" s="60" t="s">
+        <v>96</v>
+      </c>
+      <c r="I26" s="61"/>
       <c r="J26" s="17"/>
       <c r="K26" s="18"/>
       <c r="L26" s="17"/>
@@ -1532,25 +1682,29 @@
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
       <c r="B27" s="29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C27" s="35" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D27" s="36" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E27" s="37" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="H27" s="2"/>
-      <c r="I27" s="15"/>
+        <v>23</v>
+      </c>
+      <c r="H27" s="62" t="s">
+        <v>4</v>
+      </c>
+      <c r="I27" s="63" t="s">
+        <v>23</v>
+      </c>
       <c r="J27" s="2"/>
       <c r="K27" s="15"/>
       <c r="L27" s="2"/>
@@ -1559,25 +1713,29 @@
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="19"/>
       <c r="B28" s="29" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C28" s="35" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D28" s="36" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E28" s="37" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="H28" s="2"/>
-      <c r="I28" s="15"/>
+        <v>65</v>
+      </c>
+      <c r="H28" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="I28" s="63" t="s">
+        <v>87</v>
+      </c>
       <c r="J28" s="2"/>
       <c r="K28" s="15"/>
       <c r="L28" s="2"/>
@@ -1586,25 +1744,29 @@
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="19"/>
       <c r="B29" s="29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C29" s="35" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D29" s="36" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E29" s="37" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G29" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="H29" s="2"/>
-      <c r="I29" s="15"/>
+        <v>63</v>
+      </c>
+      <c r="H29" s="62" t="s">
+        <v>6</v>
+      </c>
+      <c r="I29" s="63" t="s">
+        <v>63</v>
+      </c>
       <c r="J29" s="2"/>
       <c r="K29" s="15"/>
       <c r="L29" s="2"/>
@@ -1613,25 +1775,29 @@
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="19"/>
       <c r="B30" s="29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C30" s="35" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D30" s="36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E30" s="37" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="H30" s="2"/>
-      <c r="I30" s="15"/>
+        <v>64</v>
+      </c>
+      <c r="H30" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="I30" s="63" t="s">
+        <v>97</v>
+      </c>
       <c r="J30" s="2"/>
       <c r="K30" s="15"/>
       <c r="L30" s="2"/>
@@ -1639,16 +1805,18 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="B31" s="24"/>
       <c r="C31" s="25"/>
-      <c r="D31" s="54" t="s">
-        <v>16</v>
-      </c>
-      <c r="E31" s="55"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="18"/>
+      <c r="D31" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" s="47"/>
+      <c r="F31" s="60" t="s">
+        <v>98</v>
+      </c>
+      <c r="G31" s="61"/>
       <c r="H31" s="17"/>
       <c r="I31" s="18"/>
       <c r="J31" s="17"/>
@@ -1659,19 +1827,23 @@
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="19"/>
       <c r="B32" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="D32" s="56" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32" s="57" t="s">
-        <v>58</v>
-      </c>
-      <c r="F32" s="2"/>
-      <c r="G32" s="15"/>
+        <v>50</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F32" s="62" t="s">
+        <v>4</v>
+      </c>
+      <c r="G32" s="63" t="s">
+        <v>50</v>
+      </c>
       <c r="H32" s="2"/>
       <c r="I32" s="15"/>
       <c r="J32" s="2"/>
@@ -1682,19 +1854,23 @@
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="19"/>
       <c r="B33" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="D33" s="56" t="s">
-        <v>6</v>
-      </c>
-      <c r="E33" s="57" t="s">
-        <v>59</v>
-      </c>
-      <c r="F33" s="2"/>
-      <c r="G33" s="15"/>
+        <v>51</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F33" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="G33" s="63" t="s">
+        <v>88</v>
+      </c>
       <c r="H33" s="2"/>
       <c r="I33" s="15"/>
       <c r="J33" s="2"/>
@@ -1705,19 +1881,23 @@
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="19"/>
       <c r="B34" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D34" s="56" t="s">
-        <v>7</v>
-      </c>
-      <c r="E34" s="57" t="s">
-        <v>60</v>
-      </c>
-      <c r="F34" s="2"/>
-      <c r="G34" s="15"/>
+        <v>52</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F34" s="62" t="s">
+        <v>6</v>
+      </c>
+      <c r="G34" s="63" t="s">
+        <v>52</v>
+      </c>
       <c r="H34" s="2"/>
       <c r="I34" s="15"/>
       <c r="J34" s="2"/>
@@ -1728,17 +1908,21 @@
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="20"/>
       <c r="B35" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C35" s="22"/>
-      <c r="D35" s="58" t="s">
-        <v>8</v>
-      </c>
-      <c r="E35" s="59" t="s">
-        <v>57</v>
-      </c>
-      <c r="F35" s="5"/>
-      <c r="G35" s="16"/>
+      <c r="D35" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="F35" s="64" t="s">
+        <v>7</v>
+      </c>
+      <c r="G35" s="65" t="s">
+        <v>89</v>
+      </c>
       <c r="H35" s="5"/>
       <c r="I35" s="16"/>
       <c r="J35" s="5"/>
@@ -1748,20 +1932,22 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="B36" s="49"/>
-      <c r="C36" s="49"/>
-      <c r="D36" s="50" t="s">
-        <v>16</v>
-      </c>
-      <c r="E36" s="51"/>
-      <c r="F36" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="G36" s="53"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="15"/>
+        <v>78</v>
+      </c>
+      <c r="B36" s="55"/>
+      <c r="C36" s="55"/>
+      <c r="D36" s="56" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36" s="57"/>
+      <c r="F36" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="G36" s="59"/>
+      <c r="H36" s="58" t="s">
+        <v>81</v>
+      </c>
+      <c r="I36" s="59"/>
       <c r="J36" s="2"/>
       <c r="K36" s="15"/>
       <c r="L36" s="2"/>
@@ -1770,25 +1956,29 @@
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="19"/>
       <c r="B37" s="29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C37" s="30">
         <v>8</v>
       </c>
       <c r="D37" s="36" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E37" s="37" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G37" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H37" s="2"/>
-      <c r="I37" s="15"/>
+        <v>15</v>
+      </c>
+      <c r="H37" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I37" s="12" t="s">
+        <v>15</v>
+      </c>
       <c r="J37" s="2"/>
       <c r="K37" s="15"/>
       <c r="L37" s="2"/>
@@ -1797,25 +1987,29 @@
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="19"/>
       <c r="B38" s="29" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C38" s="30" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D38" s="36" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E38" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G38" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F38" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="G38" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H38" s="2"/>
-      <c r="I38" s="15"/>
+      <c r="H38" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="I38" s="12" t="s">
+        <v>90</v>
+      </c>
       <c r="J38" s="2"/>
       <c r="K38" s="15"/>
       <c r="L38" s="2"/>
@@ -1824,25 +2018,29 @@
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="19"/>
       <c r="B39" s="29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C39" s="30" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D39" s="36" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E39" s="37" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G39" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H39" s="2"/>
-      <c r="I39" s="15"/>
+        <v>19</v>
+      </c>
+      <c r="H39" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I39" s="12" t="s">
+        <v>19</v>
+      </c>
       <c r="J39" s="2"/>
       <c r="K39" s="15"/>
       <c r="L39" s="2"/>
@@ -1851,25 +2049,29 @@
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="19"/>
       <c r="B40" s="29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C40" s="30" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D40" s="36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E40" s="37" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G40" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="H40" s="2"/>
-      <c r="I40" s="15"/>
+        <v>21</v>
+      </c>
+      <c r="H40" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I40" s="12" t="s">
+        <v>91</v>
+      </c>
       <c r="J40" s="2"/>
       <c r="K40" s="15"/>
       <c r="L40" s="2"/>
@@ -1877,161 +2079,181 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="B41" s="44"/>
-      <c r="C41" s="46"/>
-      <c r="D41" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="E41" s="45"/>
-      <c r="F41" s="54" t="s">
-        <v>76</v>
-      </c>
-      <c r="G41" s="55"/>
-      <c r="H41" s="54" t="s">
-        <v>80</v>
-      </c>
-      <c r="I41" s="55"/>
-      <c r="J41" s="17"/>
-      <c r="K41" s="18"/>
+        <v>79</v>
+      </c>
+      <c r="B41" s="48"/>
+      <c r="C41" s="53"/>
+      <c r="D41" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="E41" s="49"/>
+      <c r="F41" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="G41" s="47"/>
+      <c r="H41" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="I41" s="47"/>
+      <c r="J41" s="60" t="s">
+        <v>81</v>
+      </c>
+      <c r="K41" s="61"/>
       <c r="L41" s="17"/>
       <c r="M41" s="18"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="19"/>
       <c r="B42" s="29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C42" s="30" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D42" s="36" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E42" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="F42" s="56" t="s">
-        <v>5</v>
-      </c>
-      <c r="G42" s="57" t="s">
-        <v>62</v>
-      </c>
-      <c r="H42" s="56" t="s">
-        <v>5</v>
-      </c>
-      <c r="I42" s="57" t="s">
-        <v>62</v>
-      </c>
-      <c r="J42" s="2"/>
-      <c r="K42" s="15"/>
+        <v>53</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G42" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H42" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I42" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="J42" s="62" t="s">
+        <v>4</v>
+      </c>
+      <c r="K42" s="63" t="s">
+        <v>53</v>
+      </c>
       <c r="L42" s="2"/>
       <c r="M42" s="15"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="19"/>
       <c r="B43" s="29" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C43" s="30" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D43" s="36" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E43" s="37" t="s">
-        <v>63</v>
-      </c>
-      <c r="F43" s="56" t="s">
-        <v>6</v>
-      </c>
-      <c r="G43" s="57" t="s">
-        <v>77</v>
-      </c>
-      <c r="H43" s="56" t="s">
-        <v>6</v>
-      </c>
-      <c r="I43" s="57" t="s">
-        <v>77</v>
-      </c>
-      <c r="J43" s="2"/>
-      <c r="K43" s="15"/>
+        <v>54</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G43" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="H43" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="I43" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J43" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="K43" s="63" t="s">
+        <v>92</v>
+      </c>
       <c r="L43" s="2"/>
       <c r="M43" s="15"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="19"/>
       <c r="B44" s="29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C44" s="30" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D44" s="36" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E44" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="F44" s="56" t="s">
-        <v>7</v>
-      </c>
-      <c r="G44" s="57" t="s">
-        <v>78</v>
-      </c>
-      <c r="H44" s="56" t="s">
-        <v>7</v>
-      </c>
-      <c r="I44" s="57" t="s">
-        <v>78</v>
-      </c>
-      <c r="J44" s="2"/>
-      <c r="K44" s="15"/>
+        <v>55</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G44" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H44" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I44" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="J44" s="62" t="s">
+        <v>6</v>
+      </c>
+      <c r="K44" s="63" t="s">
+        <v>68</v>
+      </c>
       <c r="L44" s="2"/>
       <c r="M44" s="15"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="20"/>
       <c r="B45" s="31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C45" s="32"/>
       <c r="D45" s="38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E45" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="F45" s="58" t="s">
-        <v>8</v>
-      </c>
-      <c r="G45" s="59" t="s">
-        <v>79</v>
-      </c>
-      <c r="H45" s="58" t="s">
-        <v>8</v>
-      </c>
-      <c r="I45" s="59" t="s">
-        <v>79</v>
-      </c>
-      <c r="J45" s="5"/>
-      <c r="K45" s="16"/>
+        <v>49</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G45" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="H45" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I45" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="J45" s="64" t="s">
+        <v>7</v>
+      </c>
+      <c r="K45" s="65" t="s">
+        <v>93</v>
+      </c>
       <c r="L45" s="5"/>
       <c r="M45" s="16"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="26" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="B46" s="25"/>
       <c r="C46" s="25"/>
-      <c r="D46" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="E46" s="43"/>
-      <c r="F46" s="17"/>
-      <c r="G46" s="18"/>
+      <c r="D46" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="E46" s="47"/>
+      <c r="F46" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="G46" s="47"/>
       <c r="H46" s="23"/>
       <c r="I46" s="23"/>
       <c r="J46" s="17"/>
@@ -2042,19 +2264,23 @@
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="19"/>
       <c r="B47" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C47" s="21" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="F47" s="2"/>
-      <c r="G47" s="15"/>
+        <v>59</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G47" s="12" t="s">
+        <v>59</v>
+      </c>
       <c r="H47" s="11"/>
       <c r="I47" s="11"/>
       <c r="J47" s="2"/>
@@ -2065,19 +2291,23 @@
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="19"/>
       <c r="B48" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C48" s="21" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="F48" s="2"/>
-      <c r="G48" s="15"/>
+        <v>58</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G48" s="12" t="s">
+        <v>94</v>
+      </c>
       <c r="H48" s="11"/>
       <c r="I48" s="11"/>
       <c r="J48" s="2"/>
@@ -2088,19 +2318,23 @@
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="19"/>
       <c r="B49" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C49" s="21" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="F49" s="2"/>
-      <c r="G49" s="15"/>
+        <v>57</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G49" s="12" t="s">
+        <v>57</v>
+      </c>
       <c r="H49" s="11"/>
       <c r="I49" s="11"/>
       <c r="J49" s="2"/>
@@ -2111,19 +2345,23 @@
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="20"/>
       <c r="B50" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C50" s="22" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E50" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="F50" s="5"/>
-      <c r="G50" s="16"/>
+        <v>29</v>
+      </c>
+      <c r="F50" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G50" s="14" t="s">
+        <v>95</v>
+      </c>
       <c r="H50" s="13"/>
       <c r="I50" s="13"/>
       <c r="J50" s="5"/>
@@ -2132,13 +2370,15 @@
       <c r="M50" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D21:E21"/>
+  <mergeCells count="29">
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="F31:G31"/>
     <mergeCell ref="D46:E46"/>
     <mergeCell ref="H21:I21"/>
     <mergeCell ref="D31:E31"/>
@@ -2153,6 +2393,13 @@
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="F41:G41"/>
     <mergeCell ref="H41:I41"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D21:E21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>

</xml_diff>

<commit_message>
Ampliadas coordenadas de referencia para Worldclass Industries para albergar los dos tipos de formato
</commit_message>
<xml_diff>
--- a/AI_Engine/Info/Results_notes.xlsx
+++ b/AI_Engine/Info/Results_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deere-my.sharepoint.com/personal/gonzalezdiazsergio_johndeere_com/Documents/Desktop/Proyectos/Bot-Creacion-de-Pedidos/AI_Engine/Info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="13_ncr:1_{7D98053C-0B63-4673-A049-1B2D122FE4D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C733F132-CDB8-4E4C-AF89-6BE9F0B1A3D3}"/>
+  <xr:revisionPtr revIDLastSave="90" documentId="13_ncr:1_{7D98053C-0B63-4673-A049-1B2D122FE4D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AAA6836B-C774-45F5-AF75-BFD048E0CE93}"/>
   <bookViews>
-    <workbookView xWindow="13830" yWindow="3345" windowWidth="19425" windowHeight="16995" xr2:uid="{DD84187C-4454-4454-99E3-348581278C74}"/>
+    <workbookView xWindow="-14100" yWindow="5190" windowWidth="20925" windowHeight="16995" xr2:uid="{DD84187C-4454-4454-99E3-348581278C74}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="110">
   <si>
     <t>62/148</t>
   </si>
@@ -202,9 +202,6 @@
     <t>647/667</t>
   </si>
   <si>
-    <t>se ha corregido el orden de los datos, Revisar</t>
-  </si>
-  <si>
     <t>21/21</t>
   </si>
   <si>
@@ -319,9 +316,6 @@
     <t>777[7,8] agrandamiento</t>
   </si>
   <si>
-    <t>Algo raro, probar 888[7,8]</t>
-  </si>
-  <si>
     <t>0000 agrandamiento</t>
   </si>
   <si>
@@ -356,6 +350,21 @@
   </si>
   <si>
     <t>86,59</t>
+  </si>
+  <si>
+    <t>No se aplica porque agranda lo ya agrandado, probar 888[7,8]</t>
+  </si>
+  <si>
+    <t>90,55</t>
+  </si>
+  <si>
+    <t>cambios coordenadas ref</t>
+  </si>
+  <si>
+    <t>cambio orden</t>
+  </si>
+  <si>
+    <t>Orden erroneo</t>
   </si>
 </sst>
 </file>
@@ -635,52 +644,52 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -999,8 +1008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F69B5C2-6A59-4267-B787-FDE4B635DD6F}">
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1015,23 +1024,24 @@
     <col min="8" max="8" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.42578125" style="1" customWidth="1"/>
     <col min="10" max="10" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="1"/>
+    <col min="11" max="11" width="12.85546875" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="28"/>
-      <c r="D1" s="52" t="s">
+      <c r="D1" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="53"/>
-      <c r="F1" s="52" t="s">
-        <v>80</v>
-      </c>
-      <c r="G1" s="53"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="50" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" s="51"/>
       <c r="H1" s="17"/>
       <c r="I1" s="18"/>
       <c r="J1" s="17"/>
@@ -1084,7 +1094,7 @@
         <v>5</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="15"/>
@@ -1149,18 +1159,18 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" s="27"/>
       <c r="C6" s="28"/>
-      <c r="D6" s="52" t="s">
+      <c r="D6" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="53"/>
-      <c r="F6" s="54" t="s">
-        <v>80</v>
-      </c>
-      <c r="G6" s="55"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="64" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" s="65"/>
       <c r="H6" s="17"/>
       <c r="I6" s="18"/>
       <c r="J6" s="17"/>
@@ -1213,7 +1223,7 @@
         <v>5</v>
       </c>
       <c r="G8" s="43" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="15"/>
@@ -1272,26 +1282,26 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B11" s="27"/>
       <c r="C11" s="28"/>
-      <c r="D11" s="56" t="s">
+      <c r="D11" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="58"/>
-      <c r="F11" s="56" t="s">
-        <v>98</v>
-      </c>
-      <c r="G11" s="58"/>
-      <c r="H11" s="52" t="s">
+      <c r="E11" s="53"/>
+      <c r="F11" s="52" t="s">
+        <v>96</v>
+      </c>
+      <c r="G11" s="53"/>
+      <c r="H11" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="I11" s="51"/>
+      <c r="J11" s="64" t="s">
         <v>103</v>
       </c>
-      <c r="I11" s="53"/>
-      <c r="J11" s="54" t="s">
-        <v>105</v>
-      </c>
-      <c r="K11" s="55"/>
+      <c r="K11" s="65"/>
       <c r="L11" s="17"/>
       <c r="M11" s="18"/>
     </row>
@@ -1348,19 +1358,19 @@
         <v>5</v>
       </c>
       <c r="G13" s="37" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>5</v>
       </c>
       <c r="I13" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="J13" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="K13" s="43" t="s">
         <v>104</v>
-      </c>
-      <c r="J13" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="K13" s="43" t="s">
-        <v>106</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="15"/>
@@ -1377,25 +1387,25 @@
         <v>6</v>
       </c>
       <c r="E14" s="37" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F14" s="36" t="s">
         <v>6</v>
       </c>
       <c r="G14" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I14" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="H14" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="I14" s="12" t="s">
-        <v>102</v>
-      </c>
       <c r="J14" s="42" t="s">
         <v>6</v>
       </c>
       <c r="K14" s="43" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="15"/>
@@ -1416,7 +1426,7 @@
         <v>7</v>
       </c>
       <c r="G15" s="39" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H15" s="9" t="s">
         <v>7</v>
@@ -1431,20 +1441,22 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B16" s="27"/>
       <c r="C16" s="28"/>
-      <c r="D16" s="52" t="s">
+      <c r="D16" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="53"/>
-      <c r="F16" s="54" t="s">
-        <v>80</v>
-      </c>
-      <c r="G16" s="55"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="18"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="64" t="s">
+        <v>79</v>
+      </c>
+      <c r="G16" s="65"/>
+      <c r="H16" s="50" t="s">
+        <v>108</v>
+      </c>
+      <c r="I16" s="51"/>
       <c r="J16" s="17"/>
       <c r="K16" s="18"/>
       <c r="L16" s="17"/>
@@ -1470,8 +1482,12 @@
       <c r="G17" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="15"/>
+      <c r="H17" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>39</v>
+      </c>
       <c r="J17" s="2"/>
       <c r="K17" s="15"/>
       <c r="L17" s="2"/>
@@ -1495,10 +1511,14 @@
         <v>5</v>
       </c>
       <c r="G18" s="43" t="s">
-        <v>82</v>
-      </c>
-      <c r="H18" s="2"/>
-      <c r="I18" s="15"/>
+        <v>81</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>40</v>
+      </c>
       <c r="J18" s="2"/>
       <c r="K18" s="15"/>
       <c r="L18" s="2"/>
@@ -1524,8 +1544,12 @@
       <c r="G19" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="H19" s="2"/>
-      <c r="I19" s="15"/>
+      <c r="H19" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>41</v>
+      </c>
       <c r="J19" s="2"/>
       <c r="K19" s="15"/>
       <c r="L19" s="2"/>
@@ -1541,14 +1565,16 @@
         <v>7</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="F20" s="42" t="s">
         <v>7</v>
       </c>
       <c r="G20" s="43"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="15"/>
+      <c r="H20" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I20" s="12"/>
       <c r="J20" s="2"/>
       <c r="K20" s="15"/>
       <c r="L20" s="2"/>
@@ -1556,30 +1582,32 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="B21" s="59">
+        <v>73</v>
+      </c>
+      <c r="B21" s="54">
         <v>4444</v>
       </c>
-      <c r="C21" s="56"/>
-      <c r="D21" s="59">
+      <c r="C21" s="52"/>
+      <c r="D21" s="54">
         <v>5444</v>
       </c>
-      <c r="E21" s="59"/>
-      <c r="F21" s="60" t="s">
+      <c r="E21" s="54"/>
+      <c r="F21" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="G21" s="60"/>
-      <c r="H21" s="52" t="s">
+      <c r="G21" s="56"/>
+      <c r="H21" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="I21" s="53"/>
-      <c r="J21" s="54" t="s">
-        <v>80</v>
-      </c>
-      <c r="K21" s="55"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="18"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="64" t="s">
+        <v>79</v>
+      </c>
+      <c r="K21" s="65"/>
+      <c r="L21" s="50" t="s">
+        <v>108</v>
+      </c>
+      <c r="M21" s="51"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="19"/>
@@ -1613,8 +1641,12 @@
       <c r="K22" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="L22" s="2"/>
-      <c r="M22" s="15"/>
+      <c r="L22" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="M22" s="12" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="19"/>
@@ -1646,10 +1678,14 @@
         <v>5</v>
       </c>
       <c r="K23" s="43" t="s">
-        <v>83</v>
-      </c>
-      <c r="L23" s="2"/>
-      <c r="M23" s="15"/>
+        <v>82</v>
+      </c>
+      <c r="L23" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="M23" s="12" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
@@ -1683,8 +1719,12 @@
       <c r="K24" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="L24" s="2"/>
-      <c r="M24" s="15"/>
+      <c r="L24" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="M24" s="12" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="20"/>
@@ -1718,31 +1758,37 @@
       <c r="K25" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="L25" s="5"/>
-      <c r="M25" s="16"/>
+      <c r="L25" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="M25" s="14" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="B26" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="53"/>
+      <c r="D26" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="53"/>
+      <c r="F26" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="58"/>
-      <c r="D26" s="56" t="s">
-        <v>59</v>
-      </c>
-      <c r="E26" s="58"/>
-      <c r="F26" s="52" t="s">
-        <v>61</v>
-      </c>
-      <c r="G26" s="53"/>
-      <c r="H26" s="50" t="s">
-        <v>93</v>
-      </c>
-      <c r="I26" s="51"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="18"/>
+      <c r="G26" s="51"/>
+      <c r="H26" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="I26" s="63"/>
+      <c r="J26" s="50" t="s">
+        <v>108</v>
+      </c>
+      <c r="K26" s="51"/>
       <c r="L26" s="17"/>
       <c r="M26" s="18"/>
     </row>
@@ -1772,8 +1818,12 @@
       <c r="I27" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="J27" s="2"/>
-      <c r="K27" s="15"/>
+      <c r="J27" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="K27" s="12" t="s">
+        <v>23</v>
+      </c>
       <c r="L27" s="2"/>
       <c r="M27" s="15"/>
     </row>
@@ -1795,16 +1845,20 @@
         <v>5</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H28" s="46" t="s">
         <v>5</v>
       </c>
       <c r="I28" s="47" t="s">
-        <v>84</v>
-      </c>
-      <c r="J28" s="2"/>
-      <c r="K28" s="15"/>
+        <v>83</v>
+      </c>
+      <c r="J28" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="K28" s="12" t="s">
+        <v>63</v>
+      </c>
       <c r="L28" s="2"/>
       <c r="M28" s="15"/>
     </row>
@@ -1826,16 +1880,20 @@
         <v>6</v>
       </c>
       <c r="G29" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H29" s="46" t="s">
         <v>6</v>
       </c>
       <c r="I29" s="47" t="s">
-        <v>62</v>
-      </c>
-      <c r="J29" s="2"/>
-      <c r="K29" s="15"/>
+        <v>61</v>
+      </c>
+      <c r="J29" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="K29" s="12" t="s">
+        <v>61</v>
+      </c>
       <c r="L29" s="2"/>
       <c r="M29" s="15"/>
     </row>
@@ -1857,35 +1915,41 @@
         <v>7</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H30" s="46" t="s">
         <v>7</v>
       </c>
       <c r="I30" s="47" t="s">
-        <v>94</v>
-      </c>
-      <c r="J30" s="2"/>
-      <c r="K30" s="15"/>
+        <v>105</v>
+      </c>
+      <c r="J30" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="K30" s="12" t="s">
+        <v>62</v>
+      </c>
       <c r="L30" s="2"/>
       <c r="M30" s="15"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B31" s="24"/>
       <c r="C31" s="25"/>
-      <c r="D31" s="52" t="s">
+      <c r="D31" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="E31" s="53"/>
-      <c r="F31" s="50" t="s">
-        <v>95</v>
-      </c>
-      <c r="G31" s="51"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="18"/>
+      <c r="E31" s="51"/>
+      <c r="F31" s="62" t="s">
+        <v>93</v>
+      </c>
+      <c r="G31" s="63"/>
+      <c r="H31" s="50" t="s">
+        <v>108</v>
+      </c>
+      <c r="I31" s="51"/>
       <c r="J31" s="17"/>
       <c r="K31" s="18"/>
       <c r="L31" s="17"/>
@@ -1911,8 +1975,12 @@
       <c r="G32" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="H32" s="2"/>
-      <c r="I32" s="15"/>
+      <c r="H32" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I32" s="12" t="s">
+        <v>49</v>
+      </c>
       <c r="J32" s="2"/>
       <c r="K32" s="15"/>
       <c r="L32" s="2"/>
@@ -1936,10 +2004,14 @@
         <v>5</v>
       </c>
       <c r="G33" s="47" t="s">
-        <v>85</v>
-      </c>
-      <c r="H33" s="2"/>
-      <c r="I33" s="15"/>
+        <v>84</v>
+      </c>
+      <c r="H33" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="I33" s="12" t="s">
+        <v>50</v>
+      </c>
       <c r="J33" s="2"/>
       <c r="K33" s="15"/>
       <c r="L33" s="2"/>
@@ -1965,8 +2037,12 @@
       <c r="G34" s="47" t="s">
         <v>51</v>
       </c>
-      <c r="H34" s="2"/>
-      <c r="I34" s="15"/>
+      <c r="H34" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I34" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="J34" s="2"/>
       <c r="K34" s="15"/>
       <c r="L34" s="2"/>
@@ -1982,16 +2058,18 @@
         <v>7</v>
       </c>
       <c r="E35" s="14" t="s">
-        <v>48</v>
+        <v>109</v>
       </c>
       <c r="F35" s="48" t="s">
         <v>7</v>
       </c>
       <c r="G35" s="49" t="s">
-        <v>86</v>
-      </c>
-      <c r="H35" s="5"/>
-      <c r="I35" s="16"/>
+        <v>85</v>
+      </c>
+      <c r="H35" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I35" s="14"/>
       <c r="J35" s="5"/>
       <c r="K35" s="16"/>
       <c r="L35" s="5"/>
@@ -1999,24 +2077,26 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="B36" s="61"/>
-      <c r="C36" s="61"/>
-      <c r="D36" s="62" t="s">
+        <v>76</v>
+      </c>
+      <c r="B36" s="57"/>
+      <c r="C36" s="57"/>
+      <c r="D36" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="E36" s="63"/>
-      <c r="F36" s="64" t="s">
+      <c r="E36" s="59"/>
+      <c r="F36" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="G36" s="65"/>
-      <c r="H36" s="64" t="s">
-        <v>80</v>
-      </c>
-      <c r="I36" s="65"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="15"/>
+      <c r="G36" s="61"/>
+      <c r="H36" s="60" t="s">
+        <v>79</v>
+      </c>
+      <c r="I36" s="61"/>
+      <c r="J36" s="60" t="s">
+        <v>107</v>
+      </c>
+      <c r="K36" s="61"/>
       <c r="L36" s="2"/>
       <c r="M36" s="15"/>
     </row>
@@ -2046,8 +2126,12 @@
       <c r="I37" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="J37" s="2"/>
-      <c r="K37" s="15"/>
+      <c r="J37" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="K37" s="12" t="s">
+        <v>15</v>
+      </c>
       <c r="L37" s="2"/>
       <c r="M37" s="15"/>
     </row>
@@ -2075,10 +2159,14 @@
         <v>5</v>
       </c>
       <c r="I38" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="J38" s="2"/>
-      <c r="K38" s="15"/>
+        <v>86</v>
+      </c>
+      <c r="J38" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="K38" s="12" t="s">
+        <v>106</v>
+      </c>
       <c r="L38" s="2"/>
       <c r="M38" s="15"/>
     </row>
@@ -2108,8 +2196,12 @@
       <c r="I39" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J39" s="2"/>
-      <c r="K39" s="15"/>
+      <c r="J39" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="K39" s="12" t="s">
+        <v>19</v>
+      </c>
       <c r="L39" s="2"/>
       <c r="M39" s="15"/>
     </row>
@@ -2137,37 +2229,41 @@
         <v>7</v>
       </c>
       <c r="I40" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="J40" s="2"/>
-      <c r="K40" s="15"/>
+        <v>87</v>
+      </c>
+      <c r="J40" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="K40" s="12"/>
       <c r="L40" s="2"/>
       <c r="M40" s="15"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="B41" s="56"/>
-      <c r="C41" s="57"/>
-      <c r="D41" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" s="52"/>
+      <c r="C41" s="55"/>
+      <c r="D41" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="E41" s="58"/>
-      <c r="F41" s="52" t="s">
-        <v>65</v>
-      </c>
-      <c r="G41" s="53"/>
-      <c r="H41" s="52" t="s">
-        <v>69</v>
-      </c>
-      <c r="I41" s="53"/>
-      <c r="J41" s="50" t="s">
-        <v>80</v>
-      </c>
-      <c r="K41" s="51"/>
-      <c r="L41" s="17"/>
-      <c r="M41" s="18"/>
+      <c r="E41" s="53"/>
+      <c r="F41" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="G41" s="51"/>
+      <c r="H41" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="I41" s="51"/>
+      <c r="J41" s="62" t="s">
+        <v>79</v>
+      </c>
+      <c r="K41" s="63"/>
+      <c r="L41" s="50" t="s">
+        <v>108</v>
+      </c>
+      <c r="M41" s="51"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="19"/>
@@ -2201,8 +2297,12 @@
       <c r="K42" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="L42" s="2"/>
-      <c r="M42" s="15"/>
+      <c r="L42" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="M42" s="12" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="19"/>
@@ -2222,22 +2322,26 @@
         <v>5</v>
       </c>
       <c r="G43" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H43" s="8" t="s">
         <v>5</v>
       </c>
       <c r="I43" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J43" s="46" t="s">
         <v>5</v>
       </c>
       <c r="K43" s="47" t="s">
-        <v>89</v>
-      </c>
-      <c r="L43" s="2"/>
-      <c r="M43" s="15"/>
+        <v>88</v>
+      </c>
+      <c r="L43" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="M43" s="12" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="19"/>
@@ -2257,22 +2361,26 @@
         <v>6</v>
       </c>
       <c r="G44" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H44" s="8" t="s">
         <v>6</v>
       </c>
       <c r="I44" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J44" s="46" t="s">
         <v>6</v>
       </c>
       <c r="K44" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="L44" s="2"/>
-      <c r="M44" s="15"/>
+        <v>66</v>
+      </c>
+      <c r="L44" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="M44" s="12" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="20"/>
@@ -2290,37 +2398,39 @@
         <v>7</v>
       </c>
       <c r="G45" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H45" s="9" t="s">
         <v>7</v>
       </c>
       <c r="I45" s="14" t="s">
-        <v>68</v>
+        <v>109</v>
       </c>
       <c r="J45" s="48" t="s">
         <v>7</v>
       </c>
       <c r="K45" s="49" t="s">
-        <v>90</v>
-      </c>
-      <c r="L45" s="5"/>
-      <c r="M45" s="16"/>
+        <v>89</v>
+      </c>
+      <c r="L45" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="M45" s="14"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B46" s="25"/>
       <c r="C46" s="25"/>
-      <c r="D46" s="52" t="s">
+      <c r="D46" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="E46" s="53"/>
-      <c r="F46" s="52" t="s">
-        <v>80</v>
-      </c>
-      <c r="G46" s="53"/>
+      <c r="E46" s="51"/>
+      <c r="F46" s="50" t="s">
+        <v>79</v>
+      </c>
+      <c r="G46" s="51"/>
       <c r="H46" s="23"/>
       <c r="I46" s="23"/>
       <c r="J46" s="17"/>
@@ -2334,19 +2444,19 @@
         <v>4</v>
       </c>
       <c r="C47" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D47" s="8" t="s">
         <v>4</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F47" s="8" t="s">
         <v>4</v>
       </c>
       <c r="G47" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H47" s="11"/>
       <c r="I47" s="11"/>
@@ -2361,19 +2471,19 @@
         <v>5</v>
       </c>
       <c r="C48" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>5</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F48" s="8" t="s">
         <v>5</v>
       </c>
       <c r="G48" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H48" s="11"/>
       <c r="I48" s="11"/>
@@ -2388,19 +2498,19 @@
         <v>6</v>
       </c>
       <c r="C49" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D49" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F49" s="8" t="s">
         <v>6</v>
       </c>
       <c r="G49" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H49" s="11"/>
       <c r="I49" s="11"/>
@@ -2427,7 +2537,7 @@
         <v>7</v>
       </c>
       <c r="G50" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H50" s="13"/>
       <c r="I50" s="13"/>
@@ -2437,13 +2547,24 @@
       <c r="M50" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D21:E21"/>
+  <mergeCells count="38">
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="L41:M41"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="H16:I16"/>
     <mergeCell ref="D46:E46"/>
     <mergeCell ref="H21:I21"/>
     <mergeCell ref="D31:E31"/>
@@ -2459,17 +2580,12 @@
     <mergeCell ref="F41:G41"/>
     <mergeCell ref="H41:I41"/>
     <mergeCell ref="H36:I36"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D21:E21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>

</xml_diff>